<commit_message>
Added parameters and changed settings to include info of analyzed data
</commit_message>
<xml_diff>
--- a/settings/settings.xlsx
+++ b/settings/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\黄定三\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE067FB-9C8E-4A1B-A99C-C583635DF345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0643C65-1BEF-42C3-9223-01F67A905E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{7F9547E2-E7C3-45DF-8251-CDA8878506E6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>region</t>
     <phoneticPr fontId="1"/>
@@ -52,6 +52,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>1.8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>3, 1.8</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -60,6 +64,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Kyoto_kyotoshi</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>darkNumber (value)</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -68,7 +76,19 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Kanagawa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>2021/1/1,2021/1/11,2021/2/11,2021/2/23,2021/3/20,2021/4/29,2021/5/3,2021/5/4,2021/5/5,2021/7/20,2021/8/8,2021/8/9,2021/9/20,2021/9/23,2021/11/3,2021/11/23,2022/1/10,2022/2/11,2022/2/23,2022/3/21,2022/4/29,2022/5/3,2022/5/4,2022/5/5,2022/7/18,2022/8/11,2022/9/19,2022/9/23,2022/10/10,2022/11/3,2022/11/23</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CityA</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -489,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D36B5A-302C-4B28-8323-EDC2BBECE800}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:O10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -512,10 +532,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -529,52 +549,65 @@
         <v>634730</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="6"/>
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2">
+        <v>157113</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>778000</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="5"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="5"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="6"/>
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1241200</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
Removed test data, and changed darkNumber to reporting rate for easier understanding
</commit_message>
<xml_diff>
--- a/settings/settings.xlsx
+++ b/settings/settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\黄定三\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0643C65-1BEF-42C3-9223-01F67A905E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC57E8F0-C622-4E5B-BB1D-E281876E0C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{7F9547E2-E7C3-45DF-8251-CDA8878506E6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>region</t>
     <phoneticPr fontId="1"/>
@@ -48,34 +48,14 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Luxembourg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>1.8</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>3, 1.8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0, 94</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Kyoto_kyotoshi</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>darkNumber (value)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>darkNumber (start index)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>0</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -89,6 +69,14 @@
   </si>
   <si>
     <t>CityA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>reporting rate (value)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>reporting rate (start index)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -509,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D36B5A-302C-4B28-8323-EDC2BBECE800}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -532,81 +520,64 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>157113</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>634730</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
+      <c r="A3" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>157113</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>778000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1241200</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>778000</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1241200</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>